<commit_message>
Updated keywords and Also implemented Screenshot attachments in reporting
</commit_message>
<xml_diff>
--- a/EdgeQA/InputSheet/ObjectRepository.xlsx
+++ b/EdgeQA/InputSheet/ObjectRepository.xlsx
@@ -5,24 +5,25 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shreya\AI Project Workspace\Edge-Flow-QA\EdgeQA\inputSheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shreya\AI Project Workspace\Edge-Flow-QA\EdgeQA\InputSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FFDEA8-9A12-4BF9-BB9C-DB436838D2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1320F2-BAB2-4706-A38E-D7AE3DEC4E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
     <sheet name="DashboardPage" sheetId="2" r:id="rId2"/>
-    <sheet name="ExamplePage" sheetId="3" r:id="rId3"/>
+    <sheet name="GooglePage" sheetId="4" r:id="rId3"/>
+    <sheet name="ExamplePage" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>LocatorName</t>
   </si>
@@ -88,6 +89,12 @@
   </si>
   <si>
     <t>h1</t>
+  </si>
+  <si>
+    <t>searchBox</t>
+  </si>
+  <si>
+    <t>#APjFqb</t>
   </si>
 </sst>
 </file>
@@ -429,7 +436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
@@ -493,7 +500,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -572,6 +581,43 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02CFDD9E-B5C8-4F08-9024-766D3EB47341}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>

</xml_diff>